<commit_message>
Removal of invalid classes
</commit_message>
<xml_diff>
--- a/three_lens_table.xlsx
+++ b/three_lens_table.xlsx
@@ -31,13 +31,13 @@
     <t>qbe2</t>
   </si>
   <si>
+    <t>axa_adc_assumed</t>
+  </si>
+  <si>
+    <t>aspen_lpt</t>
+  </si>
+  <si>
     <t>nephila25</t>
-  </si>
-  <si>
-    <t>axa_adc_assumed</t>
-  </si>
-  <si>
-    <t>aspen_lpt</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.1934830109731649</v>
+        <v>0.1718224919819459</v>
       </c>
       <c r="C2">
         <v>0.1520909962929472</v>
@@ -431,7 +431,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.1025147025146571</v>
+        <v>0.1190503615824829</v>
       </c>
       <c r="C3">
         <v>0.1655822721874556</v>
@@ -445,13 +445,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.08759667131827932</v>
+        <v>0.09569987361192414</v>
       </c>
       <c r="C4">
-        <v>0.1574849928203699</v>
+        <v>0.08573758705076666</v>
       </c>
       <c r="D4">
-        <v>-226.7621411</v>
+        <v>-137.3742855</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -459,13 +459,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.08240751177575782</v>
+        <v>0.09478898065925606</v>
       </c>
       <c r="C5">
-        <v>0.08573758705076666</v>
+        <v>0.06706731942694223</v>
       </c>
       <c r="D5">
-        <v>-137.3742855</v>
+        <v>-142.5366911</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -473,13 +473,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.08162313851704438</v>
+        <v>0.07232465211894021</v>
       </c>
       <c r="C6">
-        <v>0.06706731942694223</v>
+        <v>0.1574849928203699</v>
       </c>
       <c r="D6">
-        <v>-142.5366911</v>
+        <v>-226.7621411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Three lens table agreed with runID 5954
</commit_message>
<xml_diff>
--- a/three_lens_table.xlsx
+++ b/three_lens_table.xlsx
@@ -417,10 +417,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.1718224919819459</v>
+        <v>0.1477845621989524</v>
       </c>
       <c r="C2">
-        <v>0.1520909962929472</v>
+        <v>0.1738072731056164</v>
       </c>
       <c r="D2">
         <v>-216.5601365</v>
@@ -431,10 +431,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.1190503615824829</v>
+        <v>0.1023952415260214</v>
       </c>
       <c r="C3">
-        <v>0.1655822721874556</v>
+        <v>0.1667320816855214</v>
       </c>
       <c r="D3">
         <v>-270.717378263</v>
@@ -445,10 +445,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.09569987361192414</v>
+        <v>0.08231148181531057</v>
       </c>
       <c r="C4">
-        <v>0.08573758705076666</v>
+        <v>0.1035517964098561</v>
       </c>
       <c r="D4">
         <v>-137.3742855</v>
@@ -459,10 +459,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.09478898065925606</v>
+        <v>0.08152802259139066</v>
       </c>
       <c r="C5">
-        <v>0.06706731942694223</v>
+        <v>0.08644468207250083</v>
       </c>
       <c r="D5">
         <v>-142.5366911</v>
@@ -473,10 +473,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.07232465211894021</v>
+        <v>0.0622064487966581</v>
       </c>
       <c r="C6">
-        <v>0.1574849928203699</v>
+        <v>0.1263389879741443</v>
       </c>
       <c r="D6">
         <v>-226.7621411</v>

</xml_diff>